<commit_message>
Added monthly statement downoad functionality.
</commit_message>
<xml_diff>
--- a/media/monthly_statements/Rajini_Level-1_Jul.xlsx
+++ b/media/monthly_statements/Rajini_Level-1_Jul.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>07/11/2018</t>
+    <t>07/24/2018</t>
   </si>
   <si>
     <t xml:space="preserve">  Franchisee Name :</t>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Sashiv Dhatrik</t>
+  </si>
+  <si>
+    <t>S138</t>
+  </si>
+  <si>
+    <t>Somiselti Roshani Sri</t>
   </si>
   <si>
     <t>Summary of this batch</t>
@@ -1254,7 +1260,7 @@
       <row>3</row>
       <rowOff>361950</rowOff>
     </from>
-    <a:ext cx="7877175" cy="1276350"/>
+    <ext cx="7877175" cy="1276350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="0" name="image1.jpg"/>
@@ -1608,8 +1614,8 @@
     </row>
     <row customHeight="1" ht="37.5" r="5" s="102" spans="1:26">
       <c r="F5" s="103" t="n"/>
-      <c r="G5" s="104" t="n"/>
-      <c r="H5" s="104" t="n"/>
+      <c r="75" s="104" t="n"/>
+      <c r="85" s="104" t="n"/>
       <c r="I5" s="6" t="n"/>
       <c r="J5" s="6" t="n"/>
       <c r="K5" s="6" t="n"/>
@@ -1625,46 +1631,46 @@
       <c r="S5" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="106" t="n"/>
+      <c r="205" s="106" t="n"/>
     </row>
     <row customHeight="1" ht="25.5" r="6" s="102" spans="1:26">
       <c r="F6" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="108" t="n"/>
-      <c r="H6" s="108" t="n"/>
-      <c r="I6" s="108" t="n"/>
+      <c r="76" s="108" t="n"/>
+      <c r="86" s="108" t="n"/>
+      <c r="96" s="108" t="n"/>
       <c r="J6" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="110" t="n"/>
-      <c r="L6" s="110" t="n"/>
-      <c r="M6" s="110" t="n"/>
+      <c r="116" s="110" t="n"/>
+      <c r="126" s="110" t="n"/>
+      <c r="136" s="110" t="n"/>
       <c r="N6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="108" t="n"/>
-      <c r="P6" s="108" t="n"/>
+      <c r="156" s="108" t="n"/>
+      <c r="166" s="108" t="n"/>
       <c r="Q6" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="110" t="n"/>
-      <c r="S6" s="110" t="n"/>
-      <c r="T6" s="112" t="n"/>
+      <c r="186" s="110" t="n"/>
+      <c r="196" s="110" t="n"/>
+      <c r="206" s="112" t="n"/>
       <c r="U6" s="19" t="n"/>
     </row>
     <row customHeight="1" ht="25.5" r="7" s="102" spans="1:26">
       <c r="F7" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="108" t="n"/>
-      <c r="H7" s="108" t="n"/>
+      <c r="77" s="108" t="n"/>
+      <c r="87" s="108" t="n"/>
       <c r="I7" s="109" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="110" t="n"/>
-      <c r="K7" s="110" t="n"/>
-      <c r="L7" s="110" t="n"/>
+      <c r="107" s="110" t="n"/>
+      <c r="117" s="110" t="n"/>
+      <c r="127" s="110" t="n"/>
       <c r="M7" s="20" t="s">
         <v>7</v>
       </c>
@@ -1677,8 +1683,8 @@
       <c r="P7" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="110" t="n"/>
-      <c r="R7" s="110" t="n"/>
+      <c r="177" s="110" t="n"/>
+      <c r="187" s="110" t="n"/>
       <c r="S7" s="20" t="s">
         <v>11</v>
       </c>
@@ -1691,68 +1697,68 @@
       <c r="F8" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="108" t="n"/>
-      <c r="H8" s="108" t="n"/>
+      <c r="78" s="108" t="n"/>
+      <c r="88" s="108" t="n"/>
       <c r="I8" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="116" t="n"/>
+      <c r="108" s="116" t="n"/>
       <c r="K8" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="118" t="n"/>
+      <c r="128" s="118" t="n"/>
       <c r="M8" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="110" t="n"/>
-      <c r="O8" s="110" t="n"/>
+      <c r="148" s="110" t="n"/>
+      <c r="158" s="110" t="n"/>
       <c r="P8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="108" t="n"/>
-      <c r="R8" s="108" t="n"/>
+      <c r="178" s="108" t="n"/>
+      <c r="188" s="108" t="n"/>
       <c r="S8" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="T8" s="112" t="n"/>
+      <c r="208" s="112" t="n"/>
     </row>
     <row customHeight="1" ht="25.5" r="9" s="102" spans="1:26">
       <c r="F9" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="108" t="n"/>
-      <c r="H9" s="108" t="n"/>
-      <c r="I9" s="108" t="n"/>
+      <c r="79" s="108" t="n"/>
+      <c r="89" s="108" t="n"/>
+      <c r="99" s="108" t="n"/>
       <c r="J9" s="121" t="n"/>
-      <c r="K9" s="108" t="n"/>
-      <c r="L9" s="108" t="n"/>
-      <c r="M9" s="108" t="n"/>
-      <c r="N9" s="108" t="n"/>
-      <c r="O9" s="108" t="n"/>
-      <c r="P9" s="108" t="n"/>
-      <c r="Q9" s="108" t="n"/>
-      <c r="R9" s="108" t="n"/>
-      <c r="S9" s="108" t="n"/>
-      <c r="T9" s="122" t="n"/>
+      <c r="119" s="108" t="n"/>
+      <c r="129" s="108" t="n"/>
+      <c r="139" s="108" t="n"/>
+      <c r="149" s="108" t="n"/>
+      <c r="159" s="108" t="n"/>
+      <c r="169" s="108" t="n"/>
+      <c r="179" s="108" t="n"/>
+      <c r="189" s="108" t="n"/>
+      <c r="199" s="108" t="n"/>
+      <c r="209" s="122" t="n"/>
     </row>
     <row customHeight="1" ht="51.75" r="10" s="102" spans="1:26">
       <c r="F10" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="124" t="n"/>
-      <c r="H10" s="124" t="n"/>
-      <c r="I10" s="124" t="n"/>
-      <c r="J10" s="124" t="n"/>
-      <c r="K10" s="124" t="n"/>
-      <c r="L10" s="124" t="n"/>
-      <c r="M10" s="124" t="n"/>
-      <c r="N10" s="124" t="n"/>
-      <c r="O10" s="124" t="n"/>
-      <c r="P10" s="124" t="n"/>
-      <c r="Q10" s="124" t="n"/>
-      <c r="R10" s="124" t="n"/>
-      <c r="S10" s="124" t="n"/>
-      <c r="T10" s="125" t="n"/>
+      <c r="710" s="124" t="n"/>
+      <c r="810" s="124" t="n"/>
+      <c r="910" s="124" t="n"/>
+      <c r="1010" s="124" t="n"/>
+      <c r="1110" s="124" t="n"/>
+      <c r="1210" s="124" t="n"/>
+      <c r="1310" s="124" t="n"/>
+      <c r="1410" s="124" t="n"/>
+      <c r="1510" s="124" t="n"/>
+      <c r="1610" s="124" t="n"/>
+      <c r="1710" s="124" t="n"/>
+      <c r="1810" s="124" t="n"/>
+      <c r="1910" s="124" t="n"/>
+      <c r="2010" s="125" t="n"/>
     </row>
     <row customHeight="1" ht="26.25" r="11" s="102" spans="1:26">
       <c r="F11" s="50" t="s">
@@ -1761,45 +1767,45 @@
       <c r="G11" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="126" t="n"/>
+      <c r="811" s="126" t="n"/>
       <c r="I11" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="104" t="n"/>
-      <c r="K11" s="104" t="n"/>
-      <c r="L11" s="104" t="n"/>
-      <c r="M11" s="104" t="n"/>
-      <c r="N11" s="126" t="n"/>
+      <c r="1011" s="104" t="n"/>
+      <c r="1111" s="104" t="n"/>
+      <c r="1211" s="104" t="n"/>
+      <c r="1311" s="104" t="n"/>
+      <c r="1411" s="126" t="n"/>
       <c r="O11" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="104" t="n"/>
+      <c r="1611" s="104" t="n"/>
       <c r="Q11" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="R11" s="128" t="n"/>
-      <c r="S11" s="128" t="n"/>
-      <c r="T11" s="129" t="n"/>
+      <c r="1811" s="128" t="n"/>
+      <c r="1911" s="128" t="n"/>
+      <c r="2011" s="129" t="n"/>
     </row>
     <row customHeight="1" ht="42" r="12" s="102" spans="1:26">
-      <c r="F12" s="130" t="n"/>
-      <c r="G12" s="131" t="n"/>
-      <c r="H12" s="125" t="n"/>
-      <c r="I12" s="131" t="n"/>
-      <c r="J12" s="124" t="n"/>
-      <c r="K12" s="124" t="n"/>
-      <c r="L12" s="124" t="n"/>
-      <c r="M12" s="124" t="n"/>
-      <c r="N12" s="125" t="n"/>
-      <c r="O12" s="124" t="n"/>
-      <c r="P12" s="124" t="n"/>
+      <c r="612" s="130" t="n"/>
+      <c r="712" s="131" t="n"/>
+      <c r="812" s="125" t="n"/>
+      <c r="912" s="131" t="n"/>
+      <c r="1012" s="124" t="n"/>
+      <c r="1112" s="124" t="n"/>
+      <c r="1212" s="124" t="n"/>
+      <c r="1312" s="124" t="n"/>
+      <c r="1412" s="125" t="n"/>
+      <c r="1512" s="124" t="n"/>
+      <c r="1612" s="124" t="n"/>
       <c r="Q12" s="50" t="s">
         <v>26</v>
       </c>
       <c r="R12" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="S12" s="129" t="n"/>
+      <c r="1912" s="129" t="n"/>
       <c r="T12" s="50" t="s">
         <v>28</v>
       </c>
@@ -1811,24 +1817,24 @@
       <c r="G13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="129" t="n"/>
+      <c r="813" s="129" t="n"/>
       <c r="I13" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="124" t="n"/>
-      <c r="K13" s="124" t="n"/>
-      <c r="L13" s="124" t="n"/>
-      <c r="M13" s="124" t="n"/>
-      <c r="N13" s="125" t="n"/>
+      <c r="1013" s="124" t="n"/>
+      <c r="1113" s="124" t="n"/>
+      <c r="1213" s="124" t="n"/>
+      <c r="1313" s="124" t="n"/>
+      <c r="1413" s="125" t="n"/>
       <c r="O13" s="55" t="s"/>
-      <c r="P13" s="129" t="n"/>
+      <c r="1613" s="129" t="n"/>
       <c r="Q13" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R13" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="S13" s="128" t="n"/>
+      <c r="1913" s="128" t="n"/>
       <c r="T13" s="55" t="s">
         <v>31</v>
       </c>
@@ -1840,24 +1846,24 @@
       <c r="G14" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="129" t="n"/>
+      <c r="814" s="129" t="n"/>
       <c r="I14" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="124" t="n"/>
-      <c r="K14" s="124" t="n"/>
-      <c r="L14" s="124" t="n"/>
-      <c r="M14" s="124" t="n"/>
-      <c r="N14" s="125" t="n"/>
+      <c r="1014" s="124" t="n"/>
+      <c r="1114" s="124" t="n"/>
+      <c r="1214" s="124" t="n"/>
+      <c r="1314" s="124" t="n"/>
+      <c r="1414" s="125" t="n"/>
       <c r="O14" s="55" t="s"/>
-      <c r="P14" s="129" t="n"/>
+      <c r="1614" s="129" t="n"/>
       <c r="Q14" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R14" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S14" s="129" t="n"/>
+      <c r="1914" s="129" t="n"/>
       <c r="T14" s="55" t="s">
         <v>31</v>
       </c>
@@ -1869,24 +1875,24 @@
       <c r="G15" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="129" t="n"/>
+      <c r="815" s="129" t="n"/>
       <c r="I15" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="124" t="n"/>
-      <c r="K15" s="124" t="n"/>
-      <c r="L15" s="124" t="n"/>
-      <c r="M15" s="124" t="n"/>
-      <c r="N15" s="125" t="n"/>
+      <c r="1015" s="124" t="n"/>
+      <c r="1115" s="124" t="n"/>
+      <c r="1215" s="124" t="n"/>
+      <c r="1315" s="124" t="n"/>
+      <c r="1415" s="125" t="n"/>
       <c r="O15" s="55" t="s"/>
-      <c r="P15" s="129" t="n"/>
+      <c r="1615" s="129" t="n"/>
       <c r="Q15" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R15" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="129" t="n"/>
+      <c r="1915" s="129" t="n"/>
       <c r="T15" s="55" t="s">
         <v>31</v>
       </c>
@@ -1898,24 +1904,24 @@
       <c r="G16" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="129" t="n"/>
+      <c r="816" s="129" t="n"/>
       <c r="I16" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="124" t="n"/>
-      <c r="K16" s="124" t="n"/>
-      <c r="L16" s="124" t="n"/>
-      <c r="M16" s="124" t="n"/>
-      <c r="N16" s="125" t="n"/>
+      <c r="1016" s="124" t="n"/>
+      <c r="1116" s="124" t="n"/>
+      <c r="1216" s="124" t="n"/>
+      <c r="1316" s="124" t="n"/>
+      <c r="1416" s="125" t="n"/>
       <c r="O16" s="55" t="s"/>
-      <c r="P16" s="129" t="n"/>
+      <c r="1616" s="129" t="n"/>
       <c r="Q16" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R16" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S16" s="129" t="n"/>
+      <c r="1916" s="129" t="n"/>
       <c r="T16" s="55" t="s">
         <v>31</v>
       </c>
@@ -1934,24 +1940,24 @@
       <c r="G17" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="129" t="n"/>
+      <c r="817" s="129" t="n"/>
       <c r="I17" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="124" t="n"/>
-      <c r="K17" s="124" t="n"/>
-      <c r="L17" s="124" t="n"/>
-      <c r="M17" s="124" t="n"/>
-      <c r="N17" s="125" t="n"/>
+      <c r="1017" s="124" t="n"/>
+      <c r="1117" s="124" t="n"/>
+      <c r="1217" s="124" t="n"/>
+      <c r="1317" s="124" t="n"/>
+      <c r="1417" s="125" t="n"/>
       <c r="O17" s="55" t="s"/>
-      <c r="P17" s="129" t="n"/>
+      <c r="1617" s="129" t="n"/>
       <c r="Q17" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R17" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="S17" s="129" t="n"/>
+      <c r="1917" s="129" t="n"/>
       <c r="T17" s="55" t="s">
         <v>40</v>
       </c>
@@ -1974,24 +1980,24 @@
       <c r="G18" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="129" t="n"/>
+      <c r="818" s="129" t="n"/>
       <c r="I18" s="132" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="124" t="n"/>
-      <c r="K18" s="124" t="n"/>
-      <c r="L18" s="124" t="n"/>
-      <c r="M18" s="124" t="n"/>
-      <c r="N18" s="125" t="n"/>
+      <c r="1018" s="124" t="n"/>
+      <c r="1118" s="124" t="n"/>
+      <c r="1218" s="124" t="n"/>
+      <c r="1318" s="124" t="n"/>
+      <c r="1418" s="125" t="n"/>
       <c r="O18" s="55" t="s"/>
-      <c r="P18" s="129" t="n"/>
+      <c r="1618" s="129" t="n"/>
       <c r="Q18" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R18" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="S18" s="129" t="n"/>
+      <c r="1918" s="129" t="n"/>
       <c r="T18" s="55" t="s">
         <v>40</v>
       </c>
@@ -2014,24 +2020,24 @@
       <c r="G19" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="129" t="n"/>
+      <c r="819" s="129" t="n"/>
       <c r="I19" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="124" t="n"/>
-      <c r="K19" s="124" t="n"/>
-      <c r="L19" s="124" t="n"/>
-      <c r="M19" s="124" t="n"/>
-      <c r="N19" s="125" t="n"/>
+      <c r="1019" s="124" t="n"/>
+      <c r="1119" s="124" t="n"/>
+      <c r="1219" s="124" t="n"/>
+      <c r="1319" s="124" t="n"/>
+      <c r="1419" s="125" t="n"/>
       <c r="O19" s="55" t="s"/>
-      <c r="P19" s="129" t="n"/>
+      <c r="1619" s="129" t="n"/>
       <c r="Q19" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R19" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S19" s="129" t="n"/>
+      <c r="1919" s="129" t="n"/>
       <c r="T19" s="55" t="s">
         <v>31</v>
       </c>
@@ -2054,24 +2060,24 @@
       <c r="G20" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="129" t="n"/>
+      <c r="820" s="129" t="n"/>
       <c r="I20" s="132" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="124" t="n"/>
-      <c r="K20" s="124" t="n"/>
-      <c r="L20" s="124" t="n"/>
-      <c r="M20" s="124" t="n"/>
-      <c r="N20" s="125" t="n"/>
+      <c r="1020" s="124" t="n"/>
+      <c r="1120" s="124" t="n"/>
+      <c r="1220" s="124" t="n"/>
+      <c r="1320" s="124" t="n"/>
+      <c r="1420" s="125" t="n"/>
       <c r="O20" s="55" t="s"/>
-      <c r="P20" s="129" t="n"/>
+      <c r="1620" s="129" t="n"/>
       <c r="Q20" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R20" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S20" s="129" t="n"/>
+      <c r="1920" s="129" t="n"/>
       <c r="T20" s="55" t="s">
         <v>31</v>
       </c>
@@ -2094,24 +2100,24 @@
       <c r="G21" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="129" t="n"/>
+      <c r="821" s="129" t="n"/>
       <c r="I21" s="132" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="124" t="n"/>
-      <c r="K21" s="124" t="n"/>
-      <c r="L21" s="124" t="n"/>
-      <c r="M21" s="124" t="n"/>
-      <c r="N21" s="125" t="n"/>
+      <c r="1021" s="124" t="n"/>
+      <c r="1121" s="124" t="n"/>
+      <c r="1221" s="124" t="n"/>
+      <c r="1321" s="124" t="n"/>
+      <c r="1421" s="125" t="n"/>
       <c r="O21" s="55" t="s"/>
-      <c r="P21" s="129" t="n"/>
+      <c r="1621" s="129" t="n"/>
       <c r="Q21" s="54" t="s">
         <v>31</v>
       </c>
       <c r="R21" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S21" s="129" t="n"/>
+      <c r="1921" s="129" t="n"/>
       <c r="T21" s="55" t="s">
         <v>31</v>
       </c>
@@ -2131,20 +2137,30 @@
       <c r="F22" s="51" t="n">
         <v>10</v>
       </c>
-      <c r="G22" s="55" t="n"/>
-      <c r="H22" s="129" t="n"/>
-      <c r="I22" s="132" t="n"/>
-      <c r="J22" s="124" t="n"/>
-      <c r="K22" s="124" t="n"/>
-      <c r="L22" s="124" t="n"/>
-      <c r="M22" s="124" t="n"/>
-      <c r="N22" s="125" t="n"/>
-      <c r="O22" s="55" t="n"/>
-      <c r="P22" s="129" t="n"/>
-      <c r="Q22" s="54" t="n"/>
-      <c r="R22" s="55" t="n"/>
-      <c r="S22" s="129" t="n"/>
-      <c r="T22" s="55" t="n"/>
+      <c r="G22" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="822" s="129" t="n"/>
+      <c r="I22" s="132" t="s">
+        <v>50</v>
+      </c>
+      <c r="1022" s="124" t="n"/>
+      <c r="1122" s="124" t="n"/>
+      <c r="1222" s="124" t="n"/>
+      <c r="1322" s="124" t="n"/>
+      <c r="1422" s="125" t="n"/>
+      <c r="O22" s="55" t="s"/>
+      <c r="1622" s="129" t="n"/>
+      <c r="Q22" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="1922" s="129" t="n"/>
+      <c r="T22" s="55" t="s">
+        <v>40</v>
+      </c>
       <c r="U22" s="57" t="n"/>
       <c r="V22" s="57" t="n"/>
       <c r="W22" s="57" t="n"/>
@@ -2162,18 +2178,18 @@
         <v>11</v>
       </c>
       <c r="G23" s="55" t="n"/>
-      <c r="H23" s="129" t="n"/>
+      <c r="823" s="129" t="n"/>
       <c r="I23" s="132" t="n"/>
-      <c r="J23" s="124" t="n"/>
-      <c r="K23" s="124" t="n"/>
-      <c r="L23" s="124" t="n"/>
-      <c r="M23" s="124" t="n"/>
-      <c r="N23" s="125" t="n"/>
+      <c r="1023" s="124" t="n"/>
+      <c r="1123" s="124" t="n"/>
+      <c r="1223" s="124" t="n"/>
+      <c r="1323" s="124" t="n"/>
+      <c r="1423" s="125" t="n"/>
       <c r="O23" s="55" t="n"/>
-      <c r="P23" s="129" t="n"/>
+      <c r="1623" s="129" t="n"/>
       <c r="Q23" s="54" t="n"/>
       <c r="R23" s="55" t="n"/>
-      <c r="S23" s="129" t="n"/>
+      <c r="1923" s="129" t="n"/>
       <c r="T23" s="55" t="n"/>
       <c r="U23" s="57" t="n"/>
       <c r="V23" s="57" t="n"/>
@@ -2192,18 +2208,18 @@
         <v>12</v>
       </c>
       <c r="G24" s="55" t="n"/>
-      <c r="H24" s="129" t="n"/>
+      <c r="824" s="129" t="n"/>
       <c r="I24" s="132" t="n"/>
-      <c r="J24" s="124" t="n"/>
-      <c r="K24" s="124" t="n"/>
-      <c r="L24" s="124" t="n"/>
-      <c r="M24" s="124" t="n"/>
-      <c r="N24" s="125" t="n"/>
+      <c r="1024" s="124" t="n"/>
+      <c r="1124" s="124" t="n"/>
+      <c r="1224" s="124" t="n"/>
+      <c r="1324" s="124" t="n"/>
+      <c r="1424" s="125" t="n"/>
       <c r="O24" s="55" t="n"/>
-      <c r="P24" s="129" t="n"/>
+      <c r="1624" s="129" t="n"/>
       <c r="Q24" s="54" t="n"/>
       <c r="R24" s="55" t="n"/>
-      <c r="S24" s="129" t="n"/>
+      <c r="1924" s="129" t="n"/>
       <c r="T24" s="55" t="n"/>
       <c r="U24" s="57" t="n"/>
       <c r="V24" s="57" t="n"/>
@@ -2222,18 +2238,18 @@
         <v>13</v>
       </c>
       <c r="G25" s="55" t="n"/>
-      <c r="H25" s="129" t="n"/>
+      <c r="825" s="129" t="n"/>
       <c r="I25" s="132" t="n"/>
-      <c r="J25" s="124" t="n"/>
-      <c r="K25" s="124" t="n"/>
-      <c r="L25" s="124" t="n"/>
-      <c r="M25" s="124" t="n"/>
-      <c r="N25" s="125" t="n"/>
+      <c r="1025" s="124" t="n"/>
+      <c r="1125" s="124" t="n"/>
+      <c r="1225" s="124" t="n"/>
+      <c r="1325" s="124" t="n"/>
+      <c r="1425" s="125" t="n"/>
       <c r="O25" s="55" t="n"/>
-      <c r="P25" s="129" t="n"/>
+      <c r="1625" s="129" t="n"/>
       <c r="Q25" s="54" t="n"/>
       <c r="R25" s="55" t="n"/>
-      <c r="S25" s="129" t="n"/>
+      <c r="1925" s="129" t="n"/>
       <c r="T25" s="55" t="n"/>
       <c r="U25" s="57" t="n"/>
       <c r="V25" s="57" t="n"/>
@@ -2252,18 +2268,18 @@
         <v>14</v>
       </c>
       <c r="G26" s="55" t="n"/>
-      <c r="H26" s="129" t="n"/>
+      <c r="826" s="129" t="n"/>
       <c r="I26" s="132" t="n"/>
-      <c r="J26" s="124" t="n"/>
-      <c r="K26" s="124" t="n"/>
-      <c r="L26" s="124" t="n"/>
-      <c r="M26" s="124" t="n"/>
-      <c r="N26" s="125" t="n"/>
+      <c r="1026" s="124" t="n"/>
+      <c r="1126" s="124" t="n"/>
+      <c r="1226" s="124" t="n"/>
+      <c r="1326" s="124" t="n"/>
+      <c r="1426" s="125" t="n"/>
       <c r="O26" s="55" t="n"/>
-      <c r="P26" s="129" t="n"/>
+      <c r="1626" s="129" t="n"/>
       <c r="Q26" s="54" t="n"/>
       <c r="R26" s="55" t="n"/>
-      <c r="S26" s="129" t="n"/>
+      <c r="1926" s="129" t="n"/>
       <c r="T26" s="55" t="n"/>
       <c r="U26" s="57" t="n"/>
       <c r="V26" s="57" t="n"/>
@@ -2282,18 +2298,18 @@
         <v>15</v>
       </c>
       <c r="G27" s="55" t="n"/>
-      <c r="H27" s="129" t="n"/>
+      <c r="827" s="129" t="n"/>
       <c r="I27" s="132" t="n"/>
-      <c r="J27" s="124" t="n"/>
-      <c r="K27" s="124" t="n"/>
-      <c r="L27" s="124" t="n"/>
-      <c r="M27" s="124" t="n"/>
-      <c r="N27" s="125" t="n"/>
+      <c r="1027" s="124" t="n"/>
+      <c r="1127" s="124" t="n"/>
+      <c r="1227" s="124" t="n"/>
+      <c r="1327" s="124" t="n"/>
+      <c r="1427" s="125" t="n"/>
       <c r="O27" s="55" t="n"/>
-      <c r="P27" s="129" t="n"/>
+      <c r="1627" s="129" t="n"/>
       <c r="Q27" s="54" t="n"/>
       <c r="R27" s="55" t="n"/>
-      <c r="S27" s="129" t="n"/>
+      <c r="1927" s="129" t="n"/>
       <c r="T27" s="55" t="n"/>
       <c r="U27" s="57" t="n"/>
       <c r="V27" s="57" t="n"/>
@@ -2310,18 +2326,18 @@
       <c r="E28" s="57" t="n"/>
       <c r="F28" s="51" t="n"/>
       <c r="G28" s="55" t="n"/>
-      <c r="H28" s="129" t="n"/>
+      <c r="828" s="129" t="n"/>
       <c r="I28" s="132" t="n"/>
-      <c r="J28" s="124" t="n"/>
-      <c r="K28" s="124" t="n"/>
-      <c r="L28" s="124" t="n"/>
-      <c r="M28" s="124" t="n"/>
-      <c r="N28" s="125" t="n"/>
+      <c r="1028" s="124" t="n"/>
+      <c r="1128" s="124" t="n"/>
+      <c r="1228" s="124" t="n"/>
+      <c r="1328" s="124" t="n"/>
+      <c r="1428" s="125" t="n"/>
       <c r="O28" s="55" t="n"/>
-      <c r="P28" s="129" t="n"/>
+      <c r="1628" s="129" t="n"/>
       <c r="Q28" s="54" t="n"/>
       <c r="R28" s="55" t="n"/>
-      <c r="S28" s="129" t="n"/>
+      <c r="1928" s="129" t="n"/>
       <c r="T28" s="55" t="n"/>
       <c r="U28" s="57" t="n"/>
       <c r="V28" s="57" t="n"/>
@@ -2338,7 +2354,7 @@
       <c r="E29" s="57" t="n"/>
       <c r="F29" s="59" t="n"/>
       <c r="G29" s="60" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H29" s="60" t="n"/>
       <c r="I29" s="60" t="n"/>
@@ -2348,9 +2364,9 @@
       <c r="M29" s="61" t="n"/>
       <c r="N29" s="63" t="n"/>
       <c r="O29" s="133" t="s">
-        <v>50</v>
-      </c>
-      <c r="P29" s="129" t="n"/>
+        <v>52</v>
+      </c>
+      <c r="1629" s="129" t="n"/>
       <c r="Q29" s="65">
         <f>COUNT(Q13:Q28)</f>
         <v/>
@@ -2359,7 +2375,7 @@
         <f>COUNT(R13:S28)</f>
         <v/>
       </c>
-      <c r="S29" s="129" t="n"/>
+      <c r="1929" s="129" t="n"/>
       <c r="T29" s="65">
         <f>COUNT(T13:T28)</f>
         <v/>
@@ -2379,7 +2395,7 @@
       <c r="E30" s="57" t="n"/>
       <c r="F30" s="68" t="n"/>
       <c r="G30" s="69" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H30" s="70" t="n"/>
       <c r="I30" s="70" t="n"/>
@@ -2388,7 +2404,7 @@
         <v/>
       </c>
       <c r="K30" s="72" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L30" s="71" t="n">
         <v>270</v>
@@ -2398,13 +2414,13 @@
         <v/>
       </c>
       <c r="N30" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="O30" s="108" t="n"/>
-      <c r="P30" s="108" t="n"/>
-      <c r="Q30" s="108" t="n"/>
-      <c r="R30" s="108" t="n"/>
-      <c r="S30" s="108" t="n"/>
+        <v>55</v>
+      </c>
+      <c r="1530" s="108" t="n"/>
+      <c r="1630" s="108" t="n"/>
+      <c r="1730" s="108" t="n"/>
+      <c r="1830" s="108" t="n"/>
+      <c r="1930" s="108" t="n"/>
       <c r="T30" s="136" t="n"/>
       <c r="U30" s="57" t="n"/>
       <c r="V30" s="57" t="n"/>
@@ -2421,7 +2437,7 @@
       <c r="E31" s="57" t="n"/>
       <c r="F31" s="68" t="n"/>
       <c r="G31" s="76" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H31" s="70" t="n"/>
       <c r="I31" s="70" t="n"/>
@@ -2430,7 +2446,7 @@
         <v/>
       </c>
       <c r="K31" s="72" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L31" s="71" t="n">
         <v>270</v>
@@ -2461,7 +2477,7 @@
       <c r="E32" s="57" t="n"/>
       <c r="F32" s="68" t="n"/>
       <c r="G32" s="69" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H32" s="79" t="n"/>
       <c r="I32" s="79" t="n"/>
@@ -2470,7 +2486,7 @@
         <v/>
       </c>
       <c r="K32" s="81" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L32" s="80" t="n">
         <v>270</v>
@@ -2501,13 +2517,13 @@
       <c r="E33" s="57" t="n"/>
       <c r="F33" s="68" t="n"/>
       <c r="G33" s="141" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="124" t="n"/>
-      <c r="I33" s="124" t="n"/>
-      <c r="J33" s="124" t="n"/>
-      <c r="K33" s="124" t="n"/>
-      <c r="L33" s="125" t="n"/>
+        <v>58</v>
+      </c>
+      <c r="833" s="124" t="n"/>
+      <c r="933" s="124" t="n"/>
+      <c r="1033" s="124" t="n"/>
+      <c r="1133" s="124" t="n"/>
+      <c r="1233" s="125" t="n"/>
       <c r="M33" s="142">
         <f>SUM(M30:M32)</f>
         <v/>
@@ -2534,13 +2550,13 @@
       <c r="E34" s="57" t="n"/>
       <c r="F34" s="68" t="n"/>
       <c r="G34" s="144" t="s">
-        <v>57</v>
-      </c>
-      <c r="H34" s="128" t="n"/>
-      <c r="I34" s="128" t="n"/>
-      <c r="J34" s="128" t="n"/>
-      <c r="K34" s="128" t="n"/>
-      <c r="L34" s="129" t="n"/>
+        <v>59</v>
+      </c>
+      <c r="834" s="128" t="n"/>
+      <c r="934" s="128" t="n"/>
+      <c r="1034" s="128" t="n"/>
+      <c r="1134" s="128" t="n"/>
+      <c r="1234" s="129" t="n"/>
       <c r="M34" s="145" t="n">
         <v>0</v>
       </c>
@@ -2566,23 +2582,23 @@
       <c r="E35" s="57" t="n"/>
       <c r="F35" s="68" t="n"/>
       <c r="G35" s="148" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" s="128" t="n"/>
-      <c r="I35" s="128" t="n"/>
-      <c r="J35" s="128" t="n"/>
-      <c r="K35" s="128" t="n"/>
-      <c r="L35" s="129" t="n"/>
+        <v>60</v>
+      </c>
+      <c r="835" s="128" t="n"/>
+      <c r="935" s="128" t="n"/>
+      <c r="1035" s="128" t="n"/>
+      <c r="1135" s="128" t="n"/>
+      <c r="1235" s="129" t="n"/>
       <c r="M35" s="149">
         <f>SUM(M33:M34)</f>
         <v/>
       </c>
       <c r="N35" s="57" t="n"/>
       <c r="O35" s="93" t="n"/>
-      <c r="P35" s="110" t="n"/>
-      <c r="Q35" s="110" t="n"/>
-      <c r="R35" s="110" t="n"/>
-      <c r="S35" s="110" t="n"/>
+      <c r="1635" s="110" t="n"/>
+      <c r="1735" s="110" t="n"/>
+      <c r="1835" s="110" t="n"/>
+      <c r="1935" s="110" t="n"/>
       <c r="T35" s="147" t="n"/>
       <c r="U35" s="57" t="n"/>
       <c r="V35" s="57" t="n"/>
@@ -2607,12 +2623,12 @@
       <c r="M36" s="57" t="n"/>
       <c r="N36" s="57" t="n"/>
       <c r="O36" s="150" t="s">
-        <v>59</v>
-      </c>
-      <c r="P36" s="118" t="n"/>
-      <c r="Q36" s="118" t="n"/>
-      <c r="R36" s="118" t="n"/>
-      <c r="S36" s="118" t="n"/>
+        <v>61</v>
+      </c>
+      <c r="1636" s="118" t="n"/>
+      <c r="1736" s="118" t="n"/>
+      <c r="1836" s="118" t="n"/>
+      <c r="1936" s="118" t="n"/>
       <c r="T36" s="138" t="n"/>
       <c r="U36" s="57" t="n"/>
       <c r="V36" s="57" t="n"/>

</xml_diff>